<commit_message>
styling and db change
</commit_message>
<xml_diff>
--- a/application/backupdb.xlsx
+++ b/application/backupdb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zach/Desktop/Aus/UWA/CITS3403/Project/Project 2/Akinator-clone/flask_auth_app/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zach/Desktop/Aus/UWA/CITS3403/Project/Project 2/Marco-Polo/application/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597365CA-C01A-2E47-816B-A855DDB37A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEBC7BA-B446-434E-B2EC-DC1D9257C8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="760" windowWidth="28600" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1418,7 +1418,7 @@
     <t>with more than 100 million people?</t>
   </si>
   <si>
-    <t>famous for Kangorros?</t>
+    <t>famous for Kangaroos?</t>
   </si>
 </sst>
 </file>
@@ -1900,7 +1900,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE201" sqref="AE201"/>
+      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>